<commit_message>
Feature: Process larger file size
</commit_message>
<xml_diff>
--- a/data/research_data.xlsx
+++ b/data/research_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jobdulo/Documents/llmapp/script_capital/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jobdulo/Documents/capty/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC41296-F312-6549-9C61-E2184F66A5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ED6176-EE25-C14A-808F-B8197F68E3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63340" yWindow="80" windowWidth="28800" windowHeight="15720" xr2:uid="{740191B5-5CDF-45C7-BDC4-AAF6DDF91110}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{740191B5-5CDF-45C7-BDC4-AAF6DDF91110}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,12 +191,6 @@
     <t>How can court reporters utilize legal transcription services?</t>
   </si>
   <si>
-    <t>Write 300-500 word article based on the below content for Capital Typing providing  legal Transcription services for court reporters.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Write 300-500 word article based on the below content for Capital Typing providing real estate lawyers with legal Transcription services. </t>
-  </si>
-  <si>
     <t>Outsourcing Transcription</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t>Data Security when Outsourcing Transcription</t>
   </si>
   <si>
-    <t>Use the responses provided to create a 500 word article for outsourcing transcription services.</t>
-  </si>
-  <si>
     <t>Exploring the benefits of outsourcing transcription services</t>
   </si>
   <si>
@@ -216,6 +207,15 @@
   </si>
   <si>
     <t>Rewrite_content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rewrite the content in 500 words. Refer to Capital Typing (www.capitaltyping.com) as a provider of real estate lawyers with legal Transcription services. </t>
+  </si>
+  <si>
+    <t>Rewrite the content in 500 words. Refer to Capital Typing (www.capitaltyping.com) as a provider of  legal Transcription services for court reporters.</t>
+  </si>
+  <si>
+    <t>Use the responses provided to create a 500 word article for Capital Typing (www.capitaltyping.com) as a provider of  outsourcing transcription services.</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E50E6D9-936C-41D0-BDB6-0969368C3E74}">
   <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP1" sqref="AP1"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AP7" sqref="AP7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -751,13 +751,13 @@
         <v>39</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>47</v>
       </c>
       <c r="AP2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AQ2" t="s">
         <v>43</v>
@@ -821,7 +821,7 @@
         <v>43</v>
       </c>
       <c r="AP3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="AQ3" t="s">
         <v>43</v>
@@ -829,31 +829,31 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
       <c r="H4" t="s">
         <v>43</v>
       </c>
       <c r="AP4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AQ4" t="s">
         <v>43</v>

</xml_diff>